<commit_message>
switch 30 on currentYear() - 30
</commit_message>
<xml_diff>
--- a/Problems 2 (1).xlsx
+++ b/Problems 2 (1).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="17771" windowHeight="9000"/>
+    <workbookView windowWidth="22188" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Var1" sheetId="1" r:id="rId1"/>
@@ -86,7 +86,7 @@
     <t>inv: self.Возраст &gt;= 18</t>
   </si>
   <si>
-    <t>inv: self.Год_выпуска &lt;= 30</t>
+    <t>inv: self.Год_выпуска &lt;= (currentYear() - 30)</t>
   </si>
   <si>
     <t>Для предыдущей задачи перестройте диаграмму классов так, чтобы можно было написать условие того, что категория ТС должна соответствать категории прав.</t>
@@ -1404,8 +1404,8 @@
   <sheetPr/>
   <dimension ref="A1:S268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="F73" sqref="F73"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="K262" sqref="K262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1435,7 +1435,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
-      <c r="M3" s="3"/>
+      <c r="M3" s="2"/>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
@@ -1568,7 +1568,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="259" spans="2:9">
+    <row r="259" spans="2:11">
       <c r="B259" s="2" t="s">
         <v>16</v>
       </c>
@@ -1579,8 +1579,10 @@
       </c>
       <c r="H259" s="2"/>
       <c r="I259" s="2"/>
-    </row>
-    <row r="260" spans="2:9">
+      <c r="J259" s="3"/>
+      <c r="K259" s="3"/>
+    </row>
+    <row r="260" spans="2:11">
       <c r="B260" s="2" t="s">
         <v>18</v>
       </c>
@@ -1591,6 +1593,8 @@
       </c>
       <c r="H260" s="2"/>
       <c r="I260" s="2"/>
+      <c r="J260" s="3"/>
+      <c r="K260" s="3"/>
     </row>
     <row r="264" spans="1:2">
       <c r="A264">
@@ -1614,7 +1618,7 @@
       <c r="E267" s="2"/>
       <c r="F267" s="2"/>
       <c r="G267" s="2"/>
-      <c r="H267" s="3"/>
+      <c r="H267" s="2"/>
     </row>
     <row r="268" spans="2:8">
       <c r="B268" s="2" t="s">
@@ -1625,7 +1629,7 @@
       <c r="E268" s="2"/>
       <c r="F268" s="2"/>
       <c r="G268" s="2"/>
-      <c r="H268" s="3"/>
+      <c r="H268" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
some useful things was deleted
</commit_message>
<xml_diff>
--- a/Problems 2 (1).xlsx
+++ b/Problems 2 (1).xlsx
@@ -275,18 +275,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -611,7 +605,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -635,16 +629,16 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -653,93 +647,92 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -847,20 +840,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>464820</xdr:colOff>
       <xdr:row>75</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>109</xdr:row>
-      <xdr:rowOff>163830</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>147320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Изображение 3"/>
+        <xdr:cNvPr id="5" name="Изображение 4"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -873,49 +866,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="617220" y="13716000"/>
-          <a:ext cx="3248025" cy="6381750"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
-      <xdr:row>110</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Изображение 4"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4937760" y="13716000"/>
+          <a:off x="464820" y="13761720"/>
           <a:ext cx="4617720" cy="6502400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -950,7 +901,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId4">
+        <a:blip r:embed="rId3">
           <a:grayscl/>
         </a:blip>
         <a:stretch>
@@ -994,7 +945,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId5"/>
+        <a:blip r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1036,7 +987,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId6"/>
+        <a:blip r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1078,7 +1029,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId7"/>
+        <a:blip r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1120,7 +1071,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId8"/>
+        <a:blip r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1404,8 +1355,8 @@
   <sheetPr/>
   <dimension ref="A1:S268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="K262" sqref="K262"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1579,8 +1530,8 @@
       </c>
       <c r="H259" s="2"/>
       <c r="I259" s="2"/>
-      <c r="J259" s="3"/>
-      <c r="K259" s="3"/>
+      <c r="J259" s="2"/>
+      <c r="K259" s="2"/>
     </row>
     <row r="260" spans="2:11">
       <c r="B260" s="2" t="s">
@@ -1593,8 +1544,8 @@
       </c>
       <c r="H260" s="2"/>
       <c r="I260" s="2"/>
-      <c r="J260" s="3"/>
-      <c r="K260" s="3"/>
+      <c r="J260" s="2"/>
+      <c r="K260" s="2"/>
     </row>
     <row r="264" spans="1:2">
       <c r="A264">

</xml_diff>